<commit_message>
Wed May 20 15:49:56 EDT 2020
</commit_message>
<xml_diff>
--- a/gantt_python/4task.xlsx
+++ b/gantt_python/4task.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="56">
   <si>
     <t>Task#</t>
   </si>
@@ -67,9 +67,6 @@
     <t>Garry</t>
   </si>
   <si>
-    <t>High</t>
-  </si>
-  <si>
     <t>t3</t>
   </si>
   <si>
@@ -112,6 +109,9 @@
     <t>GLW final review</t>
   </si>
   <si>
+    <t>t14</t>
+  </si>
+  <si>
     <t>t12</t>
   </si>
   <si>
@@ -130,7 +130,7 @@
     <t>BLU components shipping to SP</t>
   </si>
   <si>
-    <t>Apr 8, 20</t>
+    <t>May 10, 2020</t>
   </si>
   <si>
     <t>t8</t>
@@ -142,6 +142,9 @@
     <t>Mi</t>
   </si>
   <si>
+    <t>t6,t15</t>
+  </si>
+  <si>
     <t>t7</t>
   </si>
   <si>
@@ -161,6 +164,24 @@
   </si>
   <si>
     <t>t9, m2</t>
+  </si>
+  <si>
+    <t>t13</t>
+  </si>
+  <si>
+    <t>GLW 2nd revision</t>
+  </si>
+  <si>
+    <t>BOE 2nd revision</t>
+  </si>
+  <si>
+    <t>t15</t>
+  </si>
+  <si>
+    <t>Get lab access and prework done</t>
+  </si>
+  <si>
+    <t>Apr 15, 2020</t>
   </si>
 </sst>
 </file>
@@ -498,7 +519,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -567,33 +588,27 @@
         <v>21</v>
       </c>
       <c r="F3">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="E4">
         <v>20</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>13</v>
@@ -601,67 +616,70 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="E6">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="F6">
         <v>100</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="E7">
+        <v>20</v>
+      </c>
+      <c r="F7">
+        <v>100</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E7">
-        <v>14</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="I7" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="E8">
+        <v>5</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="E8">
-        <v>7</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -672,13 +690,13 @@
         <v>33</v>
       </c>
       <c r="E9">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="G9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -699,21 +717,24 @@
       <c r="B11" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="1" t="s">
         <v>38</v>
       </c>
       <c r="E11">
-        <v>7</v>
+        <v>15</v>
+      </c>
+      <c r="F11">
+        <v>80</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E12">
@@ -722,19 +743,19 @@
       <c r="G12" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="I12" s="1" t="s">
-        <v>36</v>
+      <c r="I12" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E13">
         <v>30</v>
@@ -748,10 +769,10 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E14">
         <v>7</v>
@@ -765,13 +786,73 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16">
+        <v>10</v>
+      </c>
+      <c r="F16">
+        <v>100</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E17">
+        <v>10</v>
+      </c>
+      <c r="F17">
+        <v>100</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E18">
+        <v>20</v>
+      </c>
+      <c r="F18">
+        <v>100</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>